<commit_message>
Made some edits to sound effects, shorter or made to sound appropriate
</commit_message>
<xml_diff>
--- a/Space_Hook/Assets/Sounds/Sound List.xlsx
+++ b/Space_Hook/Assets/Sounds/Sound List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni Files\2018 - 3rd Year\Semester 2\GAM20004 - Digital Prototyping Lab\Game\Space_Hook\Assets\Sounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25440AF-2924-48AA-875A-EAAF2B31B1DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72D044C-7CB7-4A8A-98BF-9A6B327B260D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="9270" xr2:uid="{53F84904-EAA4-4DB4-97B9-0E89632A93E4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Sound List</t>
   </si>
@@ -74,15 +74,9 @@
     <t>CC - No mention</t>
   </si>
   <si>
-    <t>273357__profmegavolt__hyperdrive-sound-effect-1</t>
-  </si>
-  <si>
     <t>ProfMegaVolt</t>
   </si>
   <si>
-    <t>341492__robinhood76__06515-bubble-interface-ding CC3.0 NC</t>
-  </si>
-  <si>
     <t>RobinHood76</t>
   </si>
   <si>
@@ -150,6 +144,21 @@
   </si>
   <si>
     <t>Select Object, once</t>
+  </si>
+  <si>
+    <t>Collection Chirp</t>
+  </si>
+  <si>
+    <t>used when collecting shards</t>
+  </si>
+  <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>Object Select</t>
+  </si>
+  <si>
+    <t>End of Game</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0033CF4D-23BC-40CF-A7B9-18F547718802}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,141 +615,161 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Older Alterations to Sound
</commit_message>
<xml_diff>
--- a/Space_Hook/Assets/Sounds/Sound List.xlsx
+++ b/Space_Hook/Assets/Sounds/Sound List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni Files\2018 - 3rd Year\Semester 2\GAM20004 - Digital Prototyping Lab\Game\Space_Hook\Assets\Sounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72D044C-7CB7-4A8A-98BF-9A6B327B260D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579BB9F3-13A1-4442-89AA-1E59726D0F9C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="9270" xr2:uid="{53F84904-EAA4-4DB4-97B9-0E89632A93E4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Sound List</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>End of Game</t>
+  </si>
+  <si>
+    <t>menu background on main</t>
+  </si>
+  <si>
+    <t>SOS main menu</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0033CF4D-23BC-40CF-A7B9-18F547718802}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,6 +778,23 @@
         <v>39</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>